<commit_message>
updated RR-Communication and PlanDefinition Profiles to align with the ballot changes
</commit_message>
<xml_diff>
--- a/docs/extension-rel-artifact-category.xlsx
+++ b/docs/extension-rel-artifact-category.xlsx
@@ -250,7 +250,7 @@
     <t>Type/category of one or more external resources</t>
   </si>
   <si>
-    <t>ValueSet/ext-resource-category</t>
+    <t>http://fhir.hl7.org/us/ecr/ValueSet/ext-resource-category</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -435,7 +435,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="47.64453125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="31.7734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.9609375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>

</xml_diff>